<commit_message>
Commit header and product template
</commit_message>
<xml_diff>
--- a/web/tmp/Mau_Thong_Ke_Thang.xlsx
+++ b/web/tmp/Mau_Thong_Ke_Thang.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
@@ -45,11 +45,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,52 +232,52 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -287,6 +287,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -365,6 +370,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -399,6 +405,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -574,25 +581,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
     <col min="4" max="33" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18.75">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -631,12 +639,12 @@
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
     </row>
-    <row r="2" spans="1:40" ht="18.75">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:40" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -675,235 +683,257 @@
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
     </row>
-    <row r="3" spans="1:40" ht="33" customHeight="1">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:40" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18"/>
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="5"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
     </row>
-    <row r="4" spans="1:40" ht="15" customHeight="1">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="15" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AI4" s="18" t="s">
+      <c r="AI4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="15" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6">
+    <row r="5" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="19">
         <v>2</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <v>4</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="7">
         <v>5</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <v>6</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <v>7</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="7">
         <v>8</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="7">
         <v>9</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="7">
         <v>10</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="7">
         <v>11</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="7">
         <v>12</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="7">
         <v>13</v>
       </c>
-      <c r="P5" s="10">
+      <c r="P5" s="7">
         <v>14</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="7">
         <v>15</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="7">
         <v>16</v>
       </c>
-      <c r="S5" s="10">
+      <c r="S5" s="7">
         <v>17</v>
       </c>
-      <c r="T5" s="10">
+      <c r="T5" s="7">
         <v>18</v>
       </c>
-      <c r="U5" s="10">
+      <c r="U5" s="7">
         <v>19</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="7">
         <v>20</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="7">
         <v>21</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="7">
         <v>22</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Y5" s="7">
         <v>23</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="Z5" s="7">
         <v>24</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AA5" s="7">
         <v>25</v>
       </c>
-      <c r="AB5" s="10">
+      <c r="AB5" s="7">
         <v>26</v>
       </c>
-      <c r="AC5" s="10">
+      <c r="AC5" s="7">
         <v>27</v>
       </c>
-      <c r="AD5" s="10">
+      <c r="AD5" s="7">
         <v>28</v>
       </c>
-      <c r="AE5" s="10">
+      <c r="AE5" s="7">
         <v>29</v>
       </c>
-      <c r="AF5" s="10">
+      <c r="AF5" s="7">
         <v>30</v>
       </c>
-      <c r="AG5" s="10">
+      <c r="AG5" s="7">
         <v>31</v>
       </c>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="19"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="16"/>
     </row>
-    <row r="6" spans="1:40">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="20"/>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AB6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="AG5:AG6"/>
     <mergeCell ref="C4:AG4"/>
     <mergeCell ref="AH4:AH6"/>
@@ -920,28 +950,6 @@
     <mergeCell ref="N5:N6"/>
     <mergeCell ref="O5:O6"/>
     <mergeCell ref="P5:P6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB5:AB6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -949,24 +957,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>